<commit_message>
Lasso Regression with normalization
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4EC116-F5A0-0F41-A208-594ACC569D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33620CD-B6B8-3C49-9F68-CC4D06AF1303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1920" windowWidth="27840" windowHeight="16640" xr2:uid="{FB53E5A3-0256-964B-9314-054162251140}"/>
+    <workbookView xWindow="7100" yWindow="2200" windowWidth="27840" windowHeight="16640" xr2:uid="{FB53E5A3-0256-964B-9314-054162251140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,22 @@
   </si>
   <si>
     <t>Accuracy(GB Regression)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Predicted Values(Lasso Regression + normalization)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accuracy(Lasso Regression + normalization)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Predicted Values(Ridge Regression + normalization)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accuracy(Ridge Regression + normalization)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02605EA-11A3-0541-B916-CF584A1EB961}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="L15" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -484,11 +500,13 @@
     <col min="13" max="13" width="35.1640625" customWidth="1"/>
     <col min="14" max="14" width="31.33203125" customWidth="1"/>
     <col min="15" max="15" width="22.1640625" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
-    <col min="17" max="17" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="50.83203125" customWidth="1"/>
+    <col min="17" max="17" width="41.83203125" customWidth="1"/>
+    <col min="18" max="18" width="40.6640625" customWidth="1"/>
+    <col min="19" max="19" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +552,20 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>20210201</v>
       </c>
@@ -581,8 +611,14 @@
       <c r="O2">
         <v>98.966777286012402</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <v>89.424265722820095</v>
+      </c>
+      <c r="Q2">
+        <v>99.915380695888402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>20210301</v>
       </c>
@@ -628,8 +664,14 @@
       <c r="O3">
         <v>99.977356948517496</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>85.245347256857002</v>
+      </c>
+      <c r="Q3">
+        <v>94.193753874980104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>20210401</v>
       </c>
@@ -675,8 +717,14 @@
       <c r="O4">
         <v>97.541470869337999</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>86.901971847759995</v>
+      </c>
+      <c r="Q4">
+        <v>93.442980481462399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>20210501</v>
       </c>
@@ -722,8 +770,14 @@
       <c r="O5">
         <v>97.144355855457505</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5">
+        <v>89.463154581269507</v>
+      </c>
+      <c r="Q5">
+        <v>94.171741664494206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>20210601</v>
       </c>
@@ -769,8 +823,14 @@
       <c r="O6">
         <v>96.067519438348796</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6">
+        <v>92.870833379853494</v>
+      </c>
+      <c r="Q6">
+        <v>95.252136799849794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>20210701</v>
       </c>
@@ -816,8 +876,14 @@
       <c r="O7">
         <v>94.626962967633503</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>96.396759178040895</v>
+      </c>
+      <c r="Q7">
+        <v>94.972176530089598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>20210801</v>
       </c>
@@ -863,8 +929,14 @@
       <c r="O8">
         <v>94.0073290736903</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8">
+        <v>98.712747328698498</v>
+      </c>
+      <c r="Q8">
+        <v>95.374635100191796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>20210901</v>
       </c>
@@ -910,8 +982,14 @@
       <c r="O9">
         <v>95.519598585380706</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <v>103.77907272841399</v>
+      </c>
+      <c r="Q9">
+        <v>96.989787596648696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>20211001</v>
       </c>
@@ -957,8 +1035,14 @@
       <c r="O10">
         <v>93.5660539476102</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <v>106.301350905169</v>
+      </c>
+      <c r="Q10">
+        <v>98.427176764045896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>20211101</v>
       </c>
@@ -1004,8 +1088,14 @@
       <c r="O11">
         <v>94.831671550715001</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <v>108.972637467596</v>
+      </c>
+      <c r="Q11">
+        <v>99.974896759262407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>20211201</v>
       </c>
@@ -1051,8 +1141,14 @@
       <c r="O12">
         <v>95.029082340874595</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12">
+        <v>108.97299343413</v>
+      </c>
+      <c r="Q12">
+        <v>97.297315566188004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>20220101</v>
       </c>
@@ -1098,8 +1194,14 @@
       <c r="O13">
         <v>95.483773593989298</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <v>111.617616943351</v>
+      </c>
+      <c r="Q13">
+        <v>97.910190301185807</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>20220201</v>
       </c>
@@ -1145,8 +1247,14 @@
       <c r="O14">
         <v>96.352434867692395</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>108.60726731861701</v>
+      </c>
+      <c r="Q14">
+        <v>94.441102016188907</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>20220301</v>
       </c>
@@ -1192,8 +1300,14 @@
       <c r="O15">
         <v>98.392305394936699</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <v>107.05535929926999</v>
+      </c>
+      <c r="Q15">
+        <v>93.091616781974395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>20220401</v>
       </c>
@@ -1239,8 +1353,14 @@
       <c r="O16">
         <v>98.426146998285503</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16">
+        <v>107.602555480359</v>
+      </c>
+      <c r="Q16">
+        <v>92.760823689965406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>20220501</v>
       </c>
@@ -1286,8 +1406,14 @@
       <c r="O17">
         <v>99.577436390754201</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <v>108.021300087054</v>
+      </c>
+      <c r="Q17">
+        <v>92.325897510302696</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>20220601</v>
       </c>
@@ -1333,8 +1459,14 @@
       <c r="O18">
         <v>97.018785751583295</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18">
+        <v>111.08723753240101</v>
+      </c>
+      <c r="Q18">
+        <v>94.542329814810103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>20220701</v>
       </c>
@@ -1380,8 +1512,14 @@
       <c r="O19">
         <v>98.674534966478205</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <v>114.132631897454</v>
+      </c>
+      <c r="Q19">
+        <v>95.909774703743395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>20220801</v>
       </c>
@@ -1427,8 +1565,14 @@
       <c r="O20">
         <v>99.908314268896305</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20">
+        <v>116.74875255032001</v>
+      </c>
+      <c r="Q20">
+        <v>97.290627125267207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>20220901</v>
       </c>
@@ -1474,8 +1618,14 @@
       <c r="O21">
         <v>96.949871477002503</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <v>120.62241798009801</v>
+      </c>
+      <c r="Q21">
+        <v>99.481318349918197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>20221001</v>
       </c>
@@ -1521,8 +1671,14 @@
       <c r="O22">
         <v>98.685487210793895</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22">
+        <v>120.06577162018699</v>
+      </c>
+      <c r="Q22">
+        <v>99.945190316510505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>20221101</v>
       </c>
@@ -1568,8 +1724,14 @@
       <c r="O23">
         <v>98.123605846799904</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <v>112.455097411154</v>
+      </c>
+      <c r="Q23">
+        <v>93.712581175962399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>20221201</v>
       </c>
@@ -1615,8 +1777,14 @@
       <c r="O24">
         <v>96.716192052339494</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24">
+        <v>109.112041651067</v>
+      </c>
+      <c r="Q24">
+        <v>90.926701375889905</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>20230101</v>
       </c>
@@ -1662,8 +1830,14 @@
       <c r="O25">
         <v>96.636678509490594</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <v>113.36628755078701</v>
+      </c>
+      <c r="Q25">
+        <v>94.471906292323297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>20230201</v>
       </c>
@@ -1709,8 +1883,14 @@
       <c r="O26">
         <v>98.983194220668494</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26">
+        <v>113.77421361441699</v>
+      </c>
+      <c r="Q26">
+        <v>94.811844678680899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>20230301</v>
       </c>
@@ -1756,8 +1936,14 @@
       <c r="O27">
         <v>98.268377930758007</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27">
+        <v>109.99723193538</v>
+      </c>
+      <c r="Q27">
+        <v>91.66435994615</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>20230401</v>
       </c>
@@ -1803,8 +1989,14 @@
       <c r="O28">
         <v>95.997593171337996</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28">
+        <v>109.622331985279</v>
+      </c>
+      <c r="Q28">
+        <v>89.854370479737398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>20230501</v>
       </c>
@@ -1850,8 +2042,14 @@
       <c r="O29">
         <v>97.352313079988903</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29">
+        <v>110.775691922517</v>
+      </c>
+      <c r="Q29">
+        <v>87.917215811521601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>20230601</v>
       </c>
@@ -1897,8 +2095,14 @@
       <c r="O30">
         <v>96.847890225111897</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30">
+        <v>117.55033506284801</v>
+      </c>
+      <c r="Q30">
+        <v>93.293916716546207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>20230701</v>
       </c>
@@ -1944,8 +2148,14 @@
       <c r="O31">
         <v>96.482861022049704</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31">
+        <v>117.86540934966099</v>
+      </c>
+      <c r="Q31">
+        <v>93.543975674334305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>20230801</v>
       </c>
@@ -1991,8 +2201,14 @@
       <c r="O32">
         <v>96.034519251449495</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32">
+        <v>119.106222253901</v>
+      </c>
+      <c r="Q32">
+        <v>94.528747820556902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>20230901</v>
       </c>
@@ -2038,8 +2254,14 @@
       <c r="O33">
         <v>98.653965892241501</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33">
+        <v>120.46194093141099</v>
+      </c>
+      <c r="Q33">
+        <v>94.110891352665305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>20231001</v>
       </c>
@@ -2085,8 +2307,14 @@
       <c r="O34">
         <v>98.409092261404098</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34">
+        <v>121.98171054391401</v>
+      </c>
+      <c r="Q34">
+        <v>95.298211362432994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>20231101</v>
       </c>
@@ -2132,8 +2360,14 @@
       <c r="O35">
         <v>97.670869007682498</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35">
+        <v>122.59256711488</v>
+      </c>
+      <c r="Q35">
+        <v>95.7754430585004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>20231201</v>
       </c>
@@ -2179,8 +2413,14 @@
       <c r="O36">
         <v>99.036395515006205</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36">
+        <v>124.49184498011699</v>
+      </c>
+      <c r="Q36">
+        <v>97.259253890716593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>20240101</v>
       </c>
@@ -2226,8 +2466,14 @@
       <c r="O37">
         <v>99.407421770273302</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37">
+        <v>127.46320600979401</v>
+      </c>
+      <c r="Q37">
+        <v>99.580629695151799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="C38" s="1" t="s">
         <v>6</v>
       </c>
@@ -2261,8 +2507,17 @@
       <c r="M38">
         <v>97.022580881736602</v>
       </c>
+      <c r="N38" t="s">
+        <v>6</v>
+      </c>
       <c r="O38">
         <v>97.260228876127599</v>
+      </c>
+      <c r="P38" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q38">
+        <v>95.123913938170503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Accuracy result for new target ids
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhongkun/PycharmProjects/6882-data-mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33620CD-B6B8-3C49-9F68-CC4D06AF1303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FC9D92-76C8-F84B-A5D9-74E659D4C6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="2200" windowWidth="27840" windowHeight="16640" xr2:uid="{FB53E5A3-0256-964B-9314-054162251140}"/>
+    <workbookView xWindow="2400" yWindow="1420" windowWidth="27840" windowHeight="16640" xr2:uid="{FB53E5A3-0256-964B-9314-054162251140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,10 +47,6 @@
   </si>
   <si>
     <t>Predicted values(LinearRegression)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Accuracy((LinearRegression))</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -106,11 +102,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Predicted Values(Ridge Regression + normalization)</t>
+    <t>Accuracy(LinearRegression)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Accuracy(Ridge Regression + normalization)</t>
+    <t>Predicted values(Polynomial Prediction+ normalization)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accuracy(Polynomial Prediction+ normalization)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02605EA-11A3-0541-B916-CF584A1EB961}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L15" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -491,19 +491,21 @@
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
     <col min="5" max="5" width="30.1640625" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="34.5" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" customWidth="1"/>
-    <col min="11" max="11" width="30.83203125" customWidth="1"/>
-    <col min="12" max="12" width="37.83203125" customWidth="1"/>
-    <col min="13" max="13" width="35.1640625" customWidth="1"/>
-    <col min="14" max="14" width="31.33203125" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" customWidth="1"/>
-    <col min="16" max="16" width="50.83203125" customWidth="1"/>
-    <col min="17" max="17" width="41.83203125" customWidth="1"/>
-    <col min="18" max="18" width="40.6640625" customWidth="1"/>
+    <col min="7" max="7" width="52.6640625" customWidth="1"/>
+    <col min="8" max="8" width="43" customWidth="1"/>
+    <col min="9" max="9" width="34.5" customWidth="1"/>
+    <col min="10" max="10" width="25.83203125" customWidth="1"/>
+    <col min="11" max="11" width="32" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" customWidth="1"/>
+    <col min="13" max="13" width="30.83203125" customWidth="1"/>
+    <col min="14" max="14" width="37.83203125" customWidth="1"/>
+    <col min="15" max="15" width="35.1640625" customWidth="1"/>
+    <col min="16" max="16" width="31.33203125" customWidth="1"/>
+    <col min="17" max="17" width="22.1640625" customWidth="1"/>
+    <col min="18" max="18" width="50.83203125" customWidth="1"/>
     <col min="19" max="19" width="41.83203125" customWidth="1"/>
+    <col min="20" max="20" width="40.6640625" customWidth="1"/>
+    <col min="21" max="21" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -517,52 +519,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -585,36 +587,42 @@
         <v>64.982906193151095</v>
       </c>
       <c r="G2">
+        <v>87.510650975185598</v>
+      </c>
+      <c r="H2">
+        <v>97.777263659425302</v>
+      </c>
+      <c r="I2">
         <v>87.845520833333296</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>98.151419925512101</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>89.424265722820095</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>99.915380695888402</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>72.828015421681997</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>85.5</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>95.530726256983201</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>88.575265670981096</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>98.966777286012402</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>89.424265722820095</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>99.915380695888402</v>
       </c>
     </row>
@@ -638,36 +646,42 @@
         <v>40.067343197384197</v>
       </c>
       <c r="G3">
+        <v>84.847247169212395</v>
+      </c>
+      <c r="H3">
+        <v>93.753864275372806</v>
+      </c>
+      <c r="I3">
         <v>90.183674404761902</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>99.650468955538003</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>85.245347256857002</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>94.193753874980104</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>67.410840558356497</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>92.491014194139098</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>97.799984315868301</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>90.479508038408397</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>99.977356948517496</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>85.245347256857002</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>94.193753874980104</v>
       </c>
     </row>
@@ -691,36 +705,42 @@
         <v>51.071815559071403</v>
       </c>
       <c r="G4">
+        <v>80.000087429361102</v>
+      </c>
+      <c r="H4">
+        <v>86.021599386409804</v>
+      </c>
+      <c r="I4">
         <v>91.138342261904697</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>97.998217485919099</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>86.901971847759995</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>93.442980481462399</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>63.679819588296098</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>92.491014194139098</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>99.452703434558202</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>90.713567908484293</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>97.541470869337999</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>86.901971847759995</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>93.442980481462399</v>
       </c>
     </row>
@@ -744,36 +764,42 @@
         <v>76.262151493628195</v>
       </c>
       <c r="G5">
+        <v>82.462586236712596</v>
+      </c>
+      <c r="H5">
+        <v>86.802722354434394</v>
+      </c>
+      <c r="I5">
         <v>93.219672023809494</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>98.125970551378401</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>89.463154581269507</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>94.171741664494206</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>89.374144947049302</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>92.491014194139098</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>97.358962309620097</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>92.287138062684605</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>97.144355855457505</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>89.463154581269507</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>94.171741664494206</v>
       </c>
     </row>
@@ -797,36 +823,42 @@
         <v>80.990460318699704</v>
       </c>
       <c r="G6">
+        <v>85.611473552453106</v>
+      </c>
+      <c r="H6">
+        <v>87.8066395409775</v>
+      </c>
+      <c r="I6">
         <v>96.697186904761793</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>99.176601953601903</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>92.870833379853494</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>95.252136799849794</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>96.613631606043199</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>98</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>99.487179487179404</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>93.665831452390094</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>96.067519438348796</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>92.870833379853494</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>95.252136799849794</v>
       </c>
     </row>
@@ -850,36 +882,42 @@
         <v>54.514641305694397</v>
       </c>
       <c r="G7">
+        <v>95.342039535381005</v>
+      </c>
+      <c r="H7">
+        <v>93.933043877222602</v>
+      </c>
+      <c r="I7">
         <v>98.730686904761896</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>97.271612714051102</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>96.396759178040895</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>94.972176530089598</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>116.793295846538</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>97.5</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>96.059113300492598</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>96.046367412148001</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>94.626962967633503</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>96.396759178040895</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>94.972176530089598</v>
       </c>
     </row>
@@ -903,36 +941,42 @@
         <v>77.074579030341695</v>
       </c>
       <c r="G8">
+        <v>99.964272048467905</v>
+      </c>
+      <c r="H8">
+        <v>96.583837727988296</v>
+      </c>
+      <c r="I8">
         <v>115.138451785714</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>88.755119047619004</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>98.712747328698498</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>95.374635100191796</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>125.31380700353201</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>115</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>88.8888888888888</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>109.70241440872999</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>94.0073290736903</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>98.712747328698498</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>95.374635100191796</v>
       </c>
     </row>
@@ -956,36 +1000,42 @@
         <v>57.178946126531301</v>
       </c>
       <c r="G9">
+        <v>100.726332090222</v>
+      </c>
+      <c r="H9">
+        <v>94.136758962824501</v>
+      </c>
+      <c r="I9">
         <v>116.122707738095</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>91.474104917668001</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>103.77907272841399</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>96.989787596648696</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>127.68332816176699</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>115</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>92.523364485981304</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>111.794029513642</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>95.519598585380706</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>103.77907272841399</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>96.989787596648696</v>
       </c>
     </row>
@@ -1009,36 +1059,42 @@
         <v>33.9543208648102</v>
       </c>
       <c r="G10">
+        <v>105.406160451524</v>
+      </c>
+      <c r="H10">
+        <v>97.598296714374499</v>
+      </c>
+      <c r="I10">
         <v>119.32386547618999</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>89.514939373897704</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>106.301350905169</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>98.427176764045896</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>127.13208543325401</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>115</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>93.518518518518505</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>114.94866173657999</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>93.5660539476102</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>106.301350905169</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>98.427176764045896</v>
       </c>
     </row>
@@ -1062,36 +1118,42 @@
         <v>75.059171342475295</v>
       </c>
       <c r="G11">
+        <v>111.39783552433499</v>
+      </c>
+      <c r="H11">
+        <v>97.800150895104693</v>
+      </c>
+      <c r="I11">
         <v>121.8775625</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>88.185722477064203</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>108.972637467596</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>99.974896759262407</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>113.339445718395</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>115</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>94.495412844036693</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>114.63347800971999</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>94.831671550715001</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>108.972637467596</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>99.974896759262407</v>
       </c>
     </row>
@@ -1115,36 +1177,42 @@
         <v>62.056633204993901</v>
       </c>
       <c r="G12">
+        <v>106.77871177753801</v>
+      </c>
+      <c r="H12">
+        <v>95.338135515659403</v>
+      </c>
+      <c r="I12">
         <v>122.821138095238</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>90.338269557823097</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>108.97299343413</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>97.297315566188004</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>122.573100469916</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>115</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>97.321428571428498</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>117.56742777821999</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>95.029082340874595</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>108.97299343413</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>97.297315566188004</v>
       </c>
     </row>
@@ -1168,36 +1236,42 @@
         <v>79.764943709515094</v>
       </c>
       <c r="G13">
+        <v>110.844786606558</v>
+      </c>
+      <c r="H13">
+        <v>97.232268953121505</v>
+      </c>
+      <c r="I13">
         <v>123.61775</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>91.563377192982401</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>111.617616943351</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>97.910190301185807</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>107.625889952333</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>115</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>99.122807017543806</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>119.148498102852</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>95.483773593989298</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>111.617616943351</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>97.910190301185807</v>
       </c>
     </row>
@@ -1221,36 +1295,42 @@
         <v>70.416385761495903</v>
       </c>
       <c r="G14">
+        <v>106.734418242817</v>
+      </c>
+      <c r="H14">
+        <v>92.812537602450007</v>
+      </c>
+      <c r="I14">
         <v>125.573922619047</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>90.805284679088999</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>108.60726731861701</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>94.441102016188907</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>118.14064799236399</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>115</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>100</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>119.194699902153</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>96.352434867692395</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>108.60726731861701</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>94.441102016188907</v>
       </c>
     </row>
@@ -1274,36 +1354,42 @@
         <v>65.759754111160703</v>
       </c>
       <c r="G15">
+        <v>101.316867636268</v>
+      </c>
+      <c r="H15">
+        <v>88.101624031538194</v>
+      </c>
+      <c r="I15">
         <v>126.052219047619</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>90.389374741200797</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>107.05535929926999</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>93.091616781974395</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>141.69467315508999</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>115</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>100</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>116.84884879582199</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>98.392305394936699</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>107.05535929926999</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>93.091616781974395</v>
       </c>
     </row>
@@ -1327,40 +1413,46 @@
         <v>89.187413964680601</v>
       </c>
       <c r="G16">
+        <v>104.587709957659</v>
+      </c>
+      <c r="H16">
+        <v>90.161818929016405</v>
+      </c>
+      <c r="I16">
         <v>124.206542261904</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>92.925394601806204</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>107.602555480359</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>92.760823689965406</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>135.71616376711299</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>115</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>99.137931034482705</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>117.825669481988</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>98.426146998285503</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>107.602555480359</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>92.760823689965406</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>20220501</v>
       </c>
@@ -1380,40 +1472,46 @@
         <v>63.919519720519503</v>
       </c>
       <c r="G17">
+        <v>102.812179413859</v>
+      </c>
+      <c r="H17">
+        <v>87.873657618682898</v>
+      </c>
+      <c r="I17">
         <v>126.036342261904</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>92.276630545380499</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>108.021300087054</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>92.325897510302696</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>126.776362902389</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>115</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>98.290598290598197</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>117.494399422817</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>99.577436390754201</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>108.021300087054</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>92.325897510302696</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>20220601</v>
       </c>
@@ -1433,40 +1531,46 @@
         <v>76.257501512209302</v>
       </c>
       <c r="G18">
+        <v>110.168588693232</v>
+      </c>
+      <c r="H18">
+        <v>93.760501015516795</v>
+      </c>
+      <c r="I18">
         <v>127.25706845238</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>91.696111955420406</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>111.08723753240101</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>94.542329814810103</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>121.372012180135</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>115</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>97.872340425531902</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>121.002926741889</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>97.018785751583295</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>111.08723753240101</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>94.542329814810103</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>20220701</v>
       </c>
@@ -1486,40 +1590,46 @@
         <v>67.3039780241795</v>
       </c>
       <c r="G19">
+        <v>105.722072597177</v>
+      </c>
+      <c r="H19">
+        <v>88.842077812754198</v>
+      </c>
+      <c r="I19">
         <v>126.520372619047</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>93.680359143657398</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>114.132631897454</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>95.909774703743395</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>152.72226676627301</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>115</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>96.638655462184801</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>120.57730338989001</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>98.674534966478205</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>114.132631897454</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>95.909774703743395</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>20220801</v>
       </c>
@@ -1539,40 +1649,46 @@
         <v>78.490691535003506</v>
       </c>
       <c r="G20">
+        <v>112.50215237002899</v>
+      </c>
+      <c r="H20">
+        <v>93.751793641691094</v>
+      </c>
+      <c r="I20">
         <v>126.294535714285</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>94.754553571428502</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>116.74875255032001</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>97.290627125267207</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>155.92563675238799</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>115</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>95.8333333333333</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>119.88997712267501</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>99.908314268896305</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <v>116.74875255032001</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>97.290627125267207</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>20220901</v>
       </c>
@@ -1592,40 +1708,46 @@
         <v>85.153268808002906</v>
       </c>
       <c r="G21">
+        <v>119.130899595331</v>
+      </c>
+      <c r="H21">
+        <v>99.275749662775993</v>
+      </c>
+      <c r="I21">
         <v>130.81075297619</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>90.991039186507905</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>120.62241798009801</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>99.481318349918197</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>135.98422499643499</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>115</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>95.8333333333333</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>123.660154227596</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>96.949871477002503</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>120.62241798009801</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>99.481318349918197</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>20221001</v>
       </c>
@@ -1645,40 +1767,46 @@
         <v>93.236234173123805</v>
       </c>
       <c r="G22">
+        <v>119.589344759382</v>
+      </c>
+      <c r="H22">
+        <v>99.657787299485506</v>
+      </c>
+      <c r="I22">
         <v>129.71567261904701</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>91.903606150793607</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>120.06577162018699</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>99.945190316510505</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>140.72296664935399</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>125</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>95.8333333333333</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>121.57741534704699</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>98.685487210793895</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>120.06577162018699</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>99.945190316510505</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>20221101</v>
       </c>
@@ -1698,40 +1826,46 @@
         <v>90.107307865898903</v>
       </c>
       <c r="G23">
+        <v>114.475128765305</v>
+      </c>
+      <c r="H23">
+        <v>95.395940637754606</v>
+      </c>
+      <c r="I23">
         <v>126.74876904761901</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>94.376025793650697</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>112.455097411154</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>93.712581175962399</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>128.05437653811501</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>125</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>95.8333333333333</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>122.25167298384</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>98.123605846799904</v>
       </c>
-      <c r="P23">
+      <c r="R23">
         <v>112.455097411154</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>93.712581175962399</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>20221201</v>
       </c>
@@ -1751,40 +1885,46 @@
         <v>91.160530317308798</v>
       </c>
       <c r="G24">
+        <v>110.394819500148</v>
+      </c>
+      <c r="H24">
+        <v>91.9956829167905</v>
+      </c>
+      <c r="I24">
         <v>130.370119047619</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>91.358234126984101</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>109.112041651067</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>90.926701375889905</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>85.944092917098999</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>125</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>95.8333333333333</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>123.940569537192</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>96.716192052339494</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <v>109.112041651067</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>90.926701375889905</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>20230101</v>
       </c>
@@ -1804,40 +1944,46 @@
         <v>87.391283786963498</v>
       </c>
       <c r="G25">
+        <v>126.549281821127</v>
+      </c>
+      <c r="H25">
+        <v>94.54226514906</v>
+      </c>
+      <c r="I25">
         <v>131.272077380952</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>90.606602182539703</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>113.36628755078701</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>94.471906292323297</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>95.032810762412495</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>125</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>95.8333333333333</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>124.035985788611</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>96.636678509490594</v>
       </c>
-      <c r="P25">
+      <c r="R25">
         <v>113.36628755078701</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>94.471906292323297</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>20230201</v>
       </c>
@@ -1857,40 +2003,46 @@
         <v>59.855384778962502</v>
       </c>
       <c r="G26">
+        <v>139.01200242618901</v>
+      </c>
+      <c r="H26">
+        <v>84.156664644841996</v>
+      </c>
+      <c r="I26">
         <v>130.79724404761899</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>91.002296626984105</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>113.77421361441699</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>94.811844678680899</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>174.311787333149</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>125</v>
       </c>
-      <c r="M26">
+      <c r="O26">
         <v>95.8333333333333</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <v>121.220166935197</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>98.983194220668494</v>
       </c>
-      <c r="P26">
+      <c r="R26">
         <v>113.77421361441699</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>94.811844678680899</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>20230301</v>
       </c>
@@ -1910,40 +2062,46 @@
         <v>67.156027818931193</v>
       </c>
       <c r="G27">
+        <v>120.33632895205299</v>
+      </c>
+      <c r="H27">
+        <v>99.719725873288795</v>
+      </c>
+      <c r="I27">
         <v>131.27130357142801</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>90.607247023809506</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>109.99723193538</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>91.66435994615</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>186.322542977122</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>125</v>
       </c>
-      <c r="M27">
+      <c r="O27">
         <v>95.8333333333333</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>122.07794648309</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>98.268377930758007</v>
       </c>
-      <c r="P27">
+      <c r="R27">
         <v>109.99723193538</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>91.66435994615</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>20230401</v>
       </c>
@@ -1963,40 +2121,46 @@
         <v>73.163484802202902</v>
       </c>
       <c r="G28">
+        <v>140.35254722858599</v>
+      </c>
+      <c r="H28">
+        <v>84.956928501158501</v>
+      </c>
+      <c r="I28">
         <v>131.40535119047601</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>92.2906957455113</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>109.622331985279</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>89.854370479737398</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>176.75825778877399</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>125</v>
       </c>
-      <c r="M28">
+      <c r="O28">
         <v>97.540983606557305</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>126.882936330967</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>95.997593171337996</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <v>109.622331985279</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>89.854370479737398</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>20230501</v>
       </c>
@@ -2016,40 +2180,46 @@
         <v>44.1472127397913</v>
       </c>
       <c r="G29">
+        <v>138.87508908097499</v>
+      </c>
+      <c r="H29">
+        <v>89.781675332559402</v>
+      </c>
+      <c r="I29">
         <v>134.37099404761901</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>93.356353930460998</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <v>110.775691922517</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>87.917215811521601</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>171.796208683781</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>125</v>
       </c>
-      <c r="M29">
+      <c r="O29">
         <v>99.206349206349202</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>129.33608551921299</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>97.352313079988903</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <v>110.775691922517</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>87.917215811521601</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>20230601</v>
       </c>
@@ -2069,40 +2239,46 @@
         <v>53.310636174324003</v>
       </c>
       <c r="G30">
+        <v>154.580143737962</v>
+      </c>
+      <c r="H30">
+        <v>77.317346239712407</v>
+      </c>
+      <c r="I30">
         <v>134.109952380952</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>93.563529856386893</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>117.55033506284801</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>93.293916716546207</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>155.94857329010401</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>125</v>
       </c>
-      <c r="M30">
+      <c r="O30">
         <v>99.206349206349202</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>129.971658316359</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>96.847890225111897</v>
       </c>
-      <c r="P30">
+      <c r="R30">
         <v>117.55033506284801</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>93.293916716546207</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>20230701</v>
       </c>
@@ -2122,40 +2298,46 @@
         <v>78.769229125166703</v>
       </c>
       <c r="G31">
+        <v>148.788777069785</v>
+      </c>
+      <c r="H31">
+        <v>81.913668992233994</v>
+      </c>
+      <c r="I31">
         <v>133.628678571428</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>93.945493197278793</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>117.86540934966099</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>93.543975674334305</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>155.756556253056</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>125</v>
       </c>
-      <c r="M31">
+      <c r="O31">
         <v>99.206349206349202</v>
       </c>
-      <c r="N31">
+      <c r="P31">
         <v>130.431595112217</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>96.482861022049704</v>
       </c>
-      <c r="P31">
+      <c r="R31">
         <v>117.86540934966099</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>93.543975674334305</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>20230801</v>
       </c>
@@ -2175,40 +2357,46 @@
         <v>73.605739949497902</v>
       </c>
       <c r="G32">
+        <v>151.08733991988501</v>
+      </c>
+      <c r="H32">
+        <v>80.089412761996002</v>
+      </c>
+      <c r="I32">
         <v>133.78582738095201</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>93.820771919878993</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>119.106222253901</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>94.528747820556902</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>150.35896111451299</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>125</v>
       </c>
-      <c r="M32">
+      <c r="O32">
         <v>99.206349206349202</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>130.996505743173</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>96.034519251449495</v>
       </c>
-      <c r="P32">
+      <c r="R32">
         <v>119.106222253901</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>94.528747820556902</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>20230901</v>
       </c>
@@ -2228,40 +2416,46 @@
         <v>78.098108785767593</v>
       </c>
       <c r="G33">
+        <v>150.040824454155</v>
+      </c>
+      <c r="H33">
+        <v>82.780605895190902</v>
+      </c>
+      <c r="I33">
         <v>133.52895238095201</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>95.680505952380898</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>120.46194093141099</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>94.110891352665305</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>149.85028021757799</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>125</v>
       </c>
-      <c r="M33">
+      <c r="O33">
         <v>97.65625</v>
       </c>
-      <c r="N33">
+      <c r="P33">
         <v>129.72292365793001</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>98.653965892241501</v>
       </c>
-      <c r="P33">
+      <c r="R33">
         <v>120.46194093141099</v>
       </c>
-      <c r="Q33">
+      <c r="S33">
         <v>94.110891352665305</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>20231001</v>
       </c>
@@ -2281,40 +2475,46 @@
         <v>70.740393732207295</v>
       </c>
       <c r="G34">
+        <v>148.478567873023</v>
+      </c>
+      <c r="H34">
+        <v>84.001118849200694</v>
+      </c>
+      <c r="I34">
         <v>132.99876785714201</v>
       </c>
-      <c r="H34">
+      <c r="J34">
         <v>96.094712611607093</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>121.98171054391401</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>95.298211362432994</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>177.370205464001</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>125</v>
       </c>
-      <c r="M34">
+      <c r="O34">
         <v>97.65625</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>130.036361905402</v>
       </c>
-      <c r="O34">
+      <c r="Q34">
         <v>98.409092261404098</v>
       </c>
-      <c r="P34">
+      <c r="R34">
         <v>121.98171054391401</v>
       </c>
-      <c r="Q34">
+      <c r="S34">
         <v>95.298211362432994</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>20231101</v>
       </c>
@@ -2334,40 +2534,46 @@
         <v>45.211856256471897</v>
       </c>
       <c r="G35">
+        <v>152.94317905253899</v>
+      </c>
+      <c r="H35">
+        <v>80.513141365203197</v>
+      </c>
+      <c r="I35">
         <v>133.24474404761901</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>95.902543712797595</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>122.59256711488</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>95.7754430585004</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>200.356061733259</v>
       </c>
-      <c r="L35">
+      <c r="N35">
         <v>125</v>
       </c>
-      <c r="M35">
+      <c r="O35">
         <v>97.65625</v>
       </c>
-      <c r="N35">
+      <c r="P35">
         <v>130.98128767016601</v>
       </c>
-      <c r="O35">
+      <c r="Q35">
         <v>97.670869007682498</v>
       </c>
-      <c r="P35">
+      <c r="R35">
         <v>122.59256711488</v>
       </c>
-      <c r="Q35">
+      <c r="S35">
         <v>95.7754430585004</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>20231201</v>
       </c>
@@ -2387,40 +2593,46 @@
         <v>74.302384518505704</v>
       </c>
       <c r="G36">
+        <v>143.68963975029899</v>
+      </c>
+      <c r="H36">
+        <v>87.742468945078301</v>
+      </c>
+      <c r="I36">
         <v>133.38643452380899</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>95.791848028273805</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>124.49184498011699</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>97.259253890716593</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>197.39176006415701</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>125</v>
       </c>
-      <c r="M36">
+      <c r="O36">
         <v>97.65625</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>129.23341374079101</v>
       </c>
-      <c r="O36">
+      <c r="Q36">
         <v>99.036395515006205</v>
       </c>
-      <c r="P36">
+      <c r="R36">
         <v>124.49184498011699</v>
       </c>
-      <c r="Q36">
+      <c r="S36">
         <v>97.259253890716593</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>20240101</v>
       </c>
@@ -2440,83 +2652,95 @@
         <v>80.691032834535406</v>
       </c>
       <c r="G37">
+        <v>160.61577382394501</v>
+      </c>
+      <c r="H37">
+        <v>74.518926700042499</v>
+      </c>
+      <c r="I37">
         <v>133.25822619047599</v>
       </c>
-      <c r="H37">
+      <c r="J37">
         <v>95.892010788690399</v>
       </c>
-      <c r="I37">
+      <c r="K37">
         <v>127.46320600979401</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>99.580629695151799</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>183.815746673875</v>
       </c>
-      <c r="L37">
+      <c r="N37">
         <v>125</v>
       </c>
-      <c r="M37">
+      <c r="O37">
         <v>97.65625</v>
       </c>
-      <c r="N37">
+      <c r="P37">
         <v>128.75850013405</v>
       </c>
-      <c r="O37">
+      <c r="Q37">
         <v>99.407421770273302</v>
       </c>
-      <c r="P37">
+      <c r="R37">
         <v>127.46320600979401</v>
       </c>
-      <c r="Q37">
+      <c r="S37">
         <v>99.580629695151799</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:19">
       <c r="C38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38">
         <v>74.163840790727605</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38">
         <v>69.733702040089099</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>6</v>
+      <c r="G38" t="s">
+        <v>5</v>
       </c>
       <c r="H38">
+        <v>90.234658396692694</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38">
         <v>93.442140284043703</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J38">
+      <c r="K38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L38">
         <v>95.123913938170503</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L38" t="s">
-        <v>6</v>
-      </c>
-      <c r="M38">
+      <c r="M38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38">
         <v>97.022580881736602</v>
       </c>
-      <c r="N38" t="s">
-        <v>6</v>
-      </c>
-      <c r="O38">
+      <c r="P38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q38">
         <v>97.260228876127599</v>
       </c>
-      <c r="P38" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q38">
+      <c r="R38" t="s">
+        <v>5</v>
+      </c>
+      <c r="S38">
         <v>95.123913938170503</v>
       </c>
     </row>

</xml_diff>